<commit_message>
Add organization data and update entity
</commit_message>
<xml_diff>
--- a/FwaEu.MediCare/DevelopmentData/Organizations/Organizations.xlsx
+++ b/FwaEu.MediCare/DevelopmentData/Organizations/Organizations.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652B9B49-D0C6-437C-9849-E875881370B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EF3D61-D85E-4F71-BBDF-5528EFBB6ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="13305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acteurs" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>Data type:</t>
   </si>
@@ -112,13 +112,97 @@
   </si>
   <si>
     <t>IsActive</t>
+  </si>
+  <si>
+    <t>EMS1</t>
+  </si>
+  <si>
+    <t>MEDICARE_EMS</t>
+  </si>
+  <si>
+    <t>dimitri@fwa.eu</t>
+  </si>
+  <si>
+    <t>EMS2</t>
+  </si>
+  <si>
+    <t>EMS3</t>
+  </si>
+  <si>
+    <t>soufian.boutaib@fwa.eu</t>
+  </si>
+  <si>
+    <t>mathis.rodrigues@fwa.eu</t>
+  </si>
+  <si>
+    <t>MEDICARE_EMS2</t>
+  </si>
+  <si>
+    <t>MEDICARE_EMS3</t>
+  </si>
+  <si>
+    <t>EMS4</t>
+  </si>
+  <si>
+    <t>EMS5</t>
+  </si>
+  <si>
+    <t>EMS6</t>
+  </si>
+  <si>
+    <t>EMS7</t>
+  </si>
+  <si>
+    <t>EMS8</t>
+  </si>
+  <si>
+    <t>EMS9</t>
+  </si>
+  <si>
+    <t>EMS10</t>
+  </si>
+  <si>
+    <t>EMS11</t>
+  </si>
+  <si>
+    <t>https://wild.fwa.eu/MediCare</t>
+  </si>
+  <si>
+    <t>EMS12</t>
+  </si>
+  <si>
+    <t>MEDICARE_EMS4</t>
+  </si>
+  <si>
+    <t>MEDICARE_EMS5</t>
+  </si>
+  <si>
+    <t>MEDICARE_EMS6</t>
+  </si>
+  <si>
+    <t>MEDICARE_EMS7</t>
+  </si>
+  <si>
+    <t>MEDICARE_EMS8</t>
+  </si>
+  <si>
+    <t>MEDICARE_EMS9</t>
+  </si>
+  <si>
+    <t>MEDICARE_EMS10</t>
+  </si>
+  <si>
+    <t>MEDICARE_EMS11</t>
+  </si>
+  <si>
+    <t>MEDICARE_EMS12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +230,20 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -201,10 +299,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -229,8 +328,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y89"/>
+  <dimension ref="A1:Y100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,9 +663,9 @@
     <col min="7" max="7" width="25" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
     <col min="9" max="9" width="27.42578125" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1"/>
+    <col min="10" max="10" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40.140625" customWidth="1"/>
-    <col min="12" max="12" width="28.85546875" customWidth="1"/>
+    <col min="12" max="12" width="44.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.7109375" customWidth="1"/>
     <col min="14" max="14" width="9.7109375" style="13" customWidth="1"/>
     <col min="15" max="16" width="11.42578125" style="13"/>
@@ -637,7 +750,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="8" t="b">
         <v>0</v>
@@ -652,19 +765,19 @@
         <v>0</v>
       </c>
       <c r="H10" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="8" t="b">
         <v>0</v>
@@ -769,62 +882,435 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-    </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-    </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-    </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-    </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-    </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-    </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
+      <c r="B14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="11">
+        <v>15</v>
+      </c>
+      <c r="J14" s="11">
+        <v>1</v>
+      </c>
+      <c r="K14" s="15">
+        <v>45125</v>
+      </c>
+      <c r="L14" s="11">
+        <v>5</v>
+      </c>
+      <c r="M14" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="11">
+        <v>1</v>
+      </c>
+      <c r="J15" s="11">
+        <v>2</v>
+      </c>
+      <c r="K15" s="15">
+        <v>45117</v>
+      </c>
+      <c r="L15" s="11">
+        <v>3</v>
+      </c>
+      <c r="M15" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="16">
+        <v>10</v>
+      </c>
+      <c r="J16" s="16">
+        <v>1</v>
+      </c>
+      <c r="K16" s="15">
+        <v>45126</v>
+      </c>
+      <c r="L16" s="16">
+        <v>2</v>
+      </c>
+      <c r="M16" s="16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="11">
+        <v>3</v>
+      </c>
+      <c r="J17" s="11">
+        <v>2</v>
+      </c>
+      <c r="K17" s="15">
+        <v>45125</v>
+      </c>
+      <c r="L17" s="11">
+        <v>5</v>
+      </c>
+      <c r="M17" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="11">
+        <v>1</v>
+      </c>
+      <c r="J18" s="11">
+        <v>2</v>
+      </c>
+      <c r="K18" s="15">
+        <v>45117</v>
+      </c>
+      <c r="L18" s="11">
+        <v>1</v>
+      </c>
+      <c r="M18" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="11">
+        <v>1</v>
+      </c>
+      <c r="J19" s="11">
+        <v>4</v>
+      </c>
+      <c r="K19" s="15">
+        <v>45125</v>
+      </c>
+      <c r="L19" s="11">
+        <v>1</v>
+      </c>
+      <c r="M19" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20" s="11">
+        <v>1</v>
+      </c>
+      <c r="J20" s="11">
+        <v>2</v>
+      </c>
+      <c r="K20" s="15">
+        <v>45126</v>
+      </c>
+      <c r="L20" s="11">
+        <v>1</v>
+      </c>
+      <c r="M20" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="16">
+        <v>2</v>
+      </c>
+      <c r="J21" s="16">
+        <v>3</v>
+      </c>
+      <c r="K21" s="15">
+        <v>45127</v>
+      </c>
+      <c r="L21" s="11">
+        <v>1</v>
+      </c>
+      <c r="M21" s="16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" s="11">
+        <v>15</v>
+      </c>
+      <c r="J22" s="11">
+        <v>1</v>
+      </c>
+      <c r="K22" s="15">
+        <v>45125</v>
+      </c>
+      <c r="L22" s="11">
+        <v>5</v>
+      </c>
+      <c r="M22" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="11">
+        <v>1</v>
+      </c>
+      <c r="J23" s="11">
+        <v>2</v>
+      </c>
+      <c r="K23" s="15">
+        <v>45117</v>
+      </c>
+      <c r="L23" s="11">
+        <v>3</v>
+      </c>
+      <c r="M23" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I24" s="16">
+        <v>10</v>
+      </c>
+      <c r="J24" s="16">
+        <v>1</v>
+      </c>
+      <c r="K24" s="15">
+        <v>45126</v>
+      </c>
+      <c r="L24" s="16">
+        <v>2</v>
+      </c>
+      <c r="M24" s="16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="16">
+        <v>10</v>
+      </c>
+      <c r="J25" s="16">
+        <v>1</v>
+      </c>
+      <c r="K25" s="15">
+        <v>45126</v>
+      </c>
+      <c r="L25" s="16">
+        <v>2</v>
+      </c>
+      <c r="M25" s="16" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E50" s="5"/>
@@ -986,8 +1472,73 @@
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
     </row>
+    <row r="90" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+    </row>
+    <row r="92" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+    </row>
+    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+    </row>
+    <row r="94" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+    </row>
+    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+    </row>
+    <row r="96" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+    </row>
+    <row r="97" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+    </row>
+    <row r="98" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+    </row>
+    <row r="100" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G14" r:id="rId1" xr:uid="{9C3DAB8D-AB75-42D4-A581-ED0FF1D99AA2}"/>
+    <hyperlink ref="G15" r:id="rId2" xr:uid="{ED5B57A0-4DFD-4BFF-B9A1-307B9D76FF04}"/>
+    <hyperlink ref="G16" r:id="rId3" xr:uid="{1D027453-FCC8-493A-A560-29676830531B}"/>
+    <hyperlink ref="G17" r:id="rId4" xr:uid="{5E3CC21B-4038-40DA-A140-08750FBB72E9}"/>
+    <hyperlink ref="G18" r:id="rId5" xr:uid="{F2670F25-7C64-426C-AD46-9929F7D829BC}"/>
+    <hyperlink ref="G24" r:id="rId6" xr:uid="{D3E4E18C-9090-4F8E-B7D5-1B1A7766D37E}"/>
+    <hyperlink ref="G19" r:id="rId7" xr:uid="{9B89D1A7-670E-4676-9527-F11FC6E94FD6}"/>
+    <hyperlink ref="G20" r:id="rId8" xr:uid="{8219C8E2-F244-4324-B551-9DB30ECA48B7}"/>
+    <hyperlink ref="G21" r:id="rId9" xr:uid="{30E21EC6-2D01-4CAF-A686-D13245158982}"/>
+    <hyperlink ref="G22" r:id="rId10" xr:uid="{A66B6605-9B08-4E6B-8C03-FA02320302C3}"/>
+    <hyperlink ref="G23" r:id="rId11" xr:uid="{92179908-E0FC-4443-8024-FFFAC0C67277}"/>
+    <hyperlink ref="D14" r:id="rId12" xr:uid="{D4C30BB9-28B0-424D-9CAB-9A26A94F2E2C}"/>
+    <hyperlink ref="D15" r:id="rId13" xr:uid="{610485E6-C917-46AC-8010-4BEBD4FBC283}"/>
+    <hyperlink ref="D16" r:id="rId14" xr:uid="{EF8B8A12-1DB4-4D27-90B9-84BE1D30EA45}"/>
+    <hyperlink ref="E14" r:id="rId15" xr:uid="{67295D6F-5016-4BF9-BD84-0B0689118145}"/>
+    <hyperlink ref="E15" r:id="rId16" xr:uid="{5D5134C1-2890-458E-A62E-994224B1D5E3}"/>
+    <hyperlink ref="E16" r:id="rId17" xr:uid="{5234D579-A468-465F-8C03-535D6AB565DB}"/>
+    <hyperlink ref="G25" r:id="rId18" xr:uid="{3FA4605A-1AB2-4280-A04C-454465B98289}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>